<commit_message>
Added final, laser cut version of the case.
</commit_message>
<xml_diff>
--- a/KeyboardBOM.xlsx
+++ b/KeyboardBOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Jake-Designed Planck Bill of Materials</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Ordered?</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Not Purchasing</t>
   </si>
   <si>
@@ -192,6 +189,18 @@
   </si>
   <si>
     <t>Actual Combination Total Cost (with tax and shipping):</t>
+  </si>
+  <si>
+    <t>Yes (04/12/18)</t>
+  </si>
+  <si>
+    <t>Yes (04/13/18)</t>
+  </si>
+  <si>
+    <t>Yes (04/24/18)</t>
+  </si>
+  <si>
+    <t>Yes (04/19/18)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,7 +622,7 @@
     <col min="8" max="8" width="20.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -649,13 +658,13 @@
         <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -676,16 +685,16 @@
         <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1">
         <v>8.93</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -699,20 +708,20 @@
         <v>13.66</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D13" si="0">B5*C5</f>
+        <f t="shared" ref="D5:D12" si="0">B5*C5</f>
         <v>27.32</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1">
         <v>29.74</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -733,14 +742,14 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1">
         <f>D6</f>
         <v>6.14</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -761,14 +770,14 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1">
         <f>D7</f>
         <v>4.41</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -785,17 +794,17 @@
         <v>20.95</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ref="G8:G13" si="1">D8</f>
         <v>20.95</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -816,14 +825,14 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -844,14 +853,14 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>9.99</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -872,19 +881,19 @@
         <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
         <v>21.58</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -897,22 +906,22 @@
         <v>8.17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
         <v>8.17</v>
       </c>
       <c r="H12" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -924,17 +933,17 @@
         <v>6.77</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
         <v>6.77</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -951,10 +960,10 @@
         <v>41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -971,13 +980,13 @@
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K19" s="1">
         <v>65.5</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -997,7 +1006,7 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1045,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="J23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1066,13 +1075,13 @@
         <v>24</v>
       </c>
       <c r="J24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" s="1">
         <v>62.03</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -1086,7 +1095,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="6">
         <f>SUM(G4:G13)+SUM(K19:K24)</f>

</xml_diff>